<commit_message>
Sync for the night. Update for move to work.
</commit_message>
<xml_diff>
--- a/CureReportBuilder/Sample Files/Cure Report_Template.xlsx
+++ b/CureReportBuilder/Sample Files/Cure Report_Template.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Cure Requirements</t>
   </si>
@@ -229,245 +229,6 @@
     <t>NCR</t>
   </si>
   <si>
-    <t>RAMP DOWN
-(PASS)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Temperature: 450°F +5/-10°F
-Temp. Ramp: 2°F/min +.5/-2°F/min
-Pressure: 80 psi +10/-10 psi
-Pressure Ramp: 5 psi/min +10/-5 psi/min
-Vacuum: -29 psi -3/+8 psi
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Terminate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-After 60 min
-AND
-&gt;440°F</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Temperature</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (°F)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Max:  400 | Min:  250 | Avg.: 350</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Temp. Ramp (°F/min )</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Max:  10.1 | Min: 0.5 | Avg.: 2.0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Pressure (psi)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Max:  55 | Min:  48 | Avg.: 50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Pressure Ramp (psi/min)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Max: 10 | Min:  1 | Avg.: 5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Vacuum (psi)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Max:  -25 | Min:  -29 | Avg.: -26</t>
-    </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -540,127 +301,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Temperature: 450°F +5/-450°F
-Temp. Ramp: 2°F/min +.5/-2°F/min
-Pressure: 80 psi +10/-10 psi
-Pressure Ramp: 5 psi/min +10/-5 psi/min
-Vacuum: -29 psi -3/+8 psi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Terminate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>After 60 min
-AND
-&gt;440°F</t>
-    </r>
-  </si>
-  <si>
-    <t>RAMP DOWN
-(FAIL)</t>
-  </si>
-  <si>
-    <t>Failed to Terminate</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Temperature: 450°F +5/-10°F
-Temp. Ramp: 2°F/min +.5/-2°F/min
-Pressure: 80 psi +10/-10 psi
-Pressure Ramp: 5 psi/min +10/-5 psi/min
-Vacuum: -29 psi -3/+8 psi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Terminate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>After 60 min
-AND
-&gt;440°F</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <u/>
         <sz val="14"/>
@@ -680,21 +320,6 @@
       <t xml:space="preserve">
 Omega | S#1234
 Autoclave | S#2355</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">DWELL
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>(PASS)</t>
     </r>
   </si>
   <si>
@@ -747,281 +372,6 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Temperature</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (°F)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Max:  400 | Min:  250 | Avg.: 350</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Temp. Ramp (°F/min )</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Max:  10.1 | Min: 0.5 | Avg.: 2.0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Pressure (psi)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Max:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>55</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> | Min:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">48 </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">| Avg.: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Pressure Ramp (psi/min)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Max: 10 | Min:  1 | Avg.: 5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Vacuum (inHg)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Max:  -25 | Min:  -29 | Avg.: -26</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">RAMP UP
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">(PASS)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="6"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>Start: 09-Apr-2020 11:20 PM
-End: 09-Apr-2020 10:20 PM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
         <u/>
         <sz val="14"/>
         <rFont val="Palatino Linotype"/>
@@ -1067,7 +417,7 @@
     <numFmt numFmtId="168" formatCode="h:mm\ AM/PM;@"/>
     <numFmt numFmtId="169" formatCode="[$-F0000]dd\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1221,50 +571,13 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Palatino Linotype"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Palatino Linotype"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Palatino Linotype"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Palatino Linotype"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
       <color theme="1"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
@@ -1294,20 +607,6 @@
     <font>
       <b/>
       <u/>
-      <sz val="24"/>
-      <color rgb="FF00B050"/>
-      <name val="Palatino Linotype"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color theme="1"/>
-      <name val="Palatino Linotype"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="14"/>
       <color rgb="FF00B050"/>
       <name val="Palatino Linotype"/>
@@ -1317,6 +616,13 @@
       <b/>
       <u/>
       <sz val="14"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF00B050"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
     </font>
@@ -1508,7 +814,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1673,17 +979,6 @@
       <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -1734,7 +1029,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1789,18 +1084,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1808,56 +1100,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -6115,11 +5374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="147246464"/>
-        <c:axId val="150872448"/>
+        <c:axId val="184988800"/>
+        <c:axId val="184990720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="147246464"/>
+        <c:axId val="184988800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="750"/>
@@ -6150,14 +5409,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150872448"/>
+        <c:crossAx val="184990720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
         <c:minorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150872448"/>
+        <c:axId val="184990720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150"/>
@@ -6187,7 +5446,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="147246464"/>
+        <c:crossAx val="184988800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -10349,11 +9608,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="154425984"/>
-        <c:axId val="160110848"/>
+        <c:axId val="185106816"/>
+        <c:axId val="185108736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154425984"/>
+        <c:axId val="185106816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10381,12 +9640,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="160110848"/>
+        <c:crossAx val="185108736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="160110848"/>
+        <c:axId val="185108736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="520"/>
@@ -10417,7 +9676,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154425984"/>
+        <c:crossAx val="185106816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10837,10 +10096,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:T46"/>
+  <dimension ref="A2:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10852,354 +10111,207 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
     </row>
     <row r="3" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="38" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="37" t="s">
+      <c r="L4" s="35"/>
+      <c r="M4" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
       <c r="Q4" s="27" t="s">
         <v>4</v>
       </c>
       <c r="R4" s="28"/>
     </row>
     <row r="5" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
+      <c r="A5" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
       <c r="L5" s="27"/>
       <c r="Q5" s="27"/>
     </row>
     <row r="6" spans="1:20" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="53" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="38" t="s">
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="38"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
       <c r="Q6" s="27" t="s">
         <v>4</v>
       </c>
       <c r="R6" s="28"/>
     </row>
     <row r="7" spans="1:20" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
+      <c r="A7" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" spans="1:20" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="M8" s="52"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="M8" s="32"/>
     </row>
     <row r="9" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
     </row>
     <row r="10" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
     </row>
     <row r="11" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
     </row>
     <row r="39" spans="1:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45" t="s">
+      <c r="B39" s="40"/>
+      <c r="C39" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45" t="s">
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="31" t="s">
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="168.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B40" s="44"/>
-      <c r="C40" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="34"/>
-    </row>
-    <row r="41" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="32"/>
-    </row>
-    <row r="42" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="32"/>
-    </row>
-    <row r="43" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" s="49"/>
-      <c r="C43" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="H43" s="51"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="30"/>
-    </row>
-    <row r="44" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="32"/>
-    </row>
-    <row r="45" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="32"/>
-    </row>
-    <row r="46" spans="1:10" ht="168.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="32"/>
-    </row>
+    <row r="40" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="35">
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="G42:I42"/>
+  <mergeCells count="14">
     <mergeCell ref="A2:C4"/>
     <mergeCell ref="H2:J4"/>
     <mergeCell ref="A5:C6"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:F46"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="A40:B40"/>
     <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C40:F40"/>
     <mergeCell ref="C39:F39"/>
-    <mergeCell ref="G40:I40"/>
     <mergeCell ref="G39:I39"/>
     <mergeCell ref="H5:J6"/>
     <mergeCell ref="D2:G5"/>
@@ -11208,6 +10320,7 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="M6:P6"/>
+    <mergeCell ref="A7:J7"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.57291666666666663" top="1.1145833333333299" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished up coding for post cure runs, seems to be fully functional, requires restart
</commit_message>
<xml_diff>
--- a/CureReportBuilder/Sample Files/Cure Report_Template.xlsx
+++ b/CureReportBuilder/Sample Files/Cure Report_Template.xlsx
@@ -1024,11 +1024,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="250374400"/>
-        <c:axId val="252298752"/>
+        <c:axId val="178199936"/>
+        <c:axId val="178251264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="250374400"/>
+        <c:axId val="178199936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="750"/>
@@ -1059,14 +1059,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252298752"/>
+        <c:crossAx val="178251264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
         <c:minorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252298752"/>
+        <c:axId val="178251264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150"/>
@@ -1096,7 +1096,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="250374400"/>
+        <c:crossAx val="178199936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -1167,7 +1167,7 @@
         <xdr:cNvPr id="5" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1479,7 +1479,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1490,8 +1490,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:J34"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1668,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"-,Bold"&amp;20
-&amp;26CURE REPORT&amp;R&amp;"-,Italic"&amp;9
+CURE REPORT&amp;R&amp;"-,Italic"&amp;9
 Systima Technologies
 10809 120th Ave NE
 Kirkland, WA 98033</oddHeader>

</xml_diff>

<commit_message>
Formatting changes for template and output
</commit_message>
<xml_diff>
--- a/CureReportBuilder/Sample Files/Cure Report_Template.xlsx
+++ b/CureReportBuilder/Sample Files/Cure Report_Template.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Result</t>
   </si>
@@ -240,10 +240,13 @@
     </r>
   </si>
   <si>
-    <t>Completed By: _________________________________________             Date:_________________</t>
+    <t>Date:</t>
   </si>
   <si>
-    <t xml:space="preserve">        QA Signoff: _________________________________________             Date:_________________</t>
+    <t>Completed By:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        QA Signoff:</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -760,6 +763,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -805,7 +817,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -814,9 +826,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -832,17 +841,26 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1024,11 +1042,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="178199936"/>
-        <c:axId val="178251264"/>
+        <c:axId val="219003136"/>
+        <c:axId val="219283840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178199936"/>
+        <c:axId val="219003136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="750"/>
@@ -1059,14 +1077,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178251264"/>
+        <c:crossAx val="219283840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
         <c:minorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178251264"/>
+        <c:axId val="219283840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="150"/>
@@ -1096,7 +1114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178199936"/>
+        <c:crossAx val="219003136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -1167,7 +1185,7 @@
         <xdr:cNvPr id="5" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1479,7 +1497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1490,8 +1508,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:G5"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,168 +1519,190 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:11" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="2"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="14"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
     </row>
     <row r="39" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6" t="s">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6" t="s">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="5" t="s">
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="I37:J37"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="G39:I39"/>
     <mergeCell ref="H5:J6"/>
     <mergeCell ref="D2:G5"/>
     <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="A37:J37"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="A2:C4"/>
     <mergeCell ref="H2:J4"/>
     <mergeCell ref="A5:C6"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="I34:J34"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.57291666666666663" top="1.1145833333333299" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update to template to move steps into backgroud. Added cure profile editor tab and a bunch of functionality, addded output of user run information
</commit_message>
<xml_diff>
--- a/CureReportBuilder/Sample Files/Cure Report_Template.xlsx
+++ b/CureReportBuilder/Sample Files/Cure Report_Template.xlsx
@@ -744,6 +744,20 @@
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -752,11 +766,134 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="175245952"/>
-        <c:axId val="184148736"/>
+        <c:axId val="203233152"/>
+        <c:axId val="203234688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="175245952"/>
+        <c:axId val="203233152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="514"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="203234688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="60"/>
+        <c:minorUnit val="30"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="203234688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="432.5"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="203233152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="50"/>
+        <c:minorUnit val="25"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="+mn-lt"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter>
+      <c:oddHeader>&amp;L&amp;G&amp;C&amp;"-,Bold"&amp;16CURE REPORT</c:oddHeader>
+      <c:oddFooter>&amp;RSystima Form: MF-XXXX </c:oddFooter>
+    </c:headerFooter>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.6013036134833599E-2"/>
+          <c:y val="0.14372403449568802"/>
+          <c:w val="0.81603904496832158"/>
+          <c:h val="0.71158635170603657"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="203270400"/>
+        <c:axId val="203276672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="203270400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="514"/>
@@ -787,14 +924,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184148736"/>
+        <c:crossAx val="203276672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
         <c:minorUnit val="30"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="184148736"/>
+        <c:axId val="203276672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="432.5"/>
@@ -825,12 +962,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175245952"/>
+        <c:crossAx val="203270400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
         <c:minorUnit val="25"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
@@ -849,6 +989,7 @@
     </c:extLst>
   </c:chart>
   <c:spPr>
+    <a:noFill/>
     <a:ln>
       <a:noFill/>
     </a:ln>
@@ -893,7 +1034,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 1">
+        <xdr:cNvPr id="3" name="StepChart">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
@@ -911,6 +1052,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="DataChart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1219,8 +1398,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37:J37"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>